<commit_message>
chore: importing customers informations implementation
</commit_message>
<xml_diff>
--- a/src/main/resources/files/customers.xlsx
+++ b/src/main/resources/files/customers.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -39,6 +39,9 @@
     <t>country</t>
   </si>
   <si>
+    <t>comment</t>
+  </si>
+  <si>
     <t xml:space="preserve">"Luc Artisan"</t>
   </si>
   <si>
@@ -58,6 +61,27 @@
   </si>
   <si>
     <t>"France"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaire 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaire 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaire 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaire 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaire 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaire 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaire 7</t>
   </si>
 </sst>
 </file>
@@ -102,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -110,6 +134,7 @@
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,187 +673,211 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2">
         <v>95160</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2">
         <v>95160</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2">
         <v>95160</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2">
         <v>95160</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2">
         <v>95160</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="2">
         <v>95160</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F8" s="2">
         <v>95160</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: ignore missing informations during import from file
</commit_message>
<xml_diff>
--- a/src/main/resources/files/customers.xlsx
+++ b/src/main/resources/files/customers.xlsx
@@ -13,36 +13,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>Prénom(s)</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Téléphone</t>
-  </si>
-  <si>
-    <t>Siteweb</t>
-  </si>
-  <si>
-    <t>Adresse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code Postal</t>
-  </si>
-  <si>
-    <t>Ville</t>
-  </si>
-  <si>
-    <t>Pays</t>
-  </si>
-  <si>
-    <t>Commentaires</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <si>
+    <t xml:space="preserve">Nom </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Prénom(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Téléphone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siteweb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code Postal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ville </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pays </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaires </t>
   </si>
   <si>
     <t>Artisan</t>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t xml:space="preserve">Commentaire 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -162,6 +165,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table3" ref="A1:J9">
+  <autoFilter ref="A1:J9"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Nom "/>
+    <tableColumn id="2" name=" Prénom(s)"/>
+    <tableColumn id="3" name="Email "/>
+    <tableColumn id="4" name="Téléphone "/>
+    <tableColumn id="5" name="Siteweb "/>
+    <tableColumn id="6" name="Adresse "/>
+    <tableColumn id="7" name="Code Postal "/>
+    <tableColumn id="8" name="Ville "/>
+    <tableColumn id="9" name="Pays "/>
+    <tableColumn id="10" name="Commentaires "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium24" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
@@ -662,6 +684,14 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="2" max="2" width="12.28125"/>
+    <col bestFit="1" min="4" max="4" width="12.28125"/>
+    <col bestFit="1" min="5" max="5" width="10.140625"/>
+    <col bestFit="1" min="6" max="6" width="10.00390625"/>
+    <col bestFit="1" min="7" max="7" width="13.421875"/>
+    <col bestFit="1" min="10" max="10" width="15.8515625"/>
+  </cols>
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="1" t="s">
@@ -917,6 +947,11 @@
       </c>
       <c r="J8" s="4" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -924,5 +959,8 @@
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: allow some nullable values when importing/crupdating customers
</commit_message>
<xml_diff>
--- a/src/main/resources/files/customers.xlsx
+++ b/src/main/resources/files/customers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afryan/IdeaProjects/bpartners-api/src/main/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F932D8A8-7AEC-D64A-9159-51E7157B77B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F1F3BB-BAFF-6F42-ADB6-FFD817E6941B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Nom</t>
   </si>
@@ -77,9 +77,6 @@
     <t>test@email.com</t>
   </si>
   <si>
-    <t>0612345678</t>
-  </si>
-  <si>
     <t>FR</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>test+other+email@email.com</t>
+  </si>
+  <si>
+    <t>test+test@email.com</t>
   </si>
 </sst>
 </file>
@@ -218,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,9 +227,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -640,7 +638,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -692,14 +690,14 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
+      <c r="D2" s="3">
+        <v>612345678</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s">
@@ -712,21 +710,21 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
@@ -736,18 +734,16 @@
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D4" s="3">
         <v>612345678</v>
@@ -761,22 +757,22 @@
         <v>10</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="3" t="s">
@@ -789,127 +785,127 @@
         <v>10</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6">
+        <v>26</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3">
         <v>75000</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="6"/>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="6">
+      <c r="D7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3">
         <v>75000</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="6"/>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="6" t="s">
+      <c r="D8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="3">
+        <v>75000</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="6">
-        <v>75000</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="6"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="3">
+        <v>75000</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="6">
-        <v>75000</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="6"/>
+      <c r="J9" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{E48622D3-3F43-2C42-A6A1-8E71B9C115C8}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{9B0FCB87-6845-5043-B8FD-3A7079AA0638}"/>
-    <hyperlink ref="C4" r:id="rId3" display="mailto:test@email.com" xr:uid="{1F7AC3FA-A387-724A-8B8E-D0CF29158FD1}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{1F7AC3FA-A387-724A-8B8E-D0CF29158FD1}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{ADC8D78D-A89C-9E4C-A3D6-83FED66169D8}"/>
     <hyperlink ref="C7" r:id="rId5" xr:uid="{A9D1E25F-43F7-6E4F-9E3D-D99C8529C80D}"/>
     <hyperlink ref="C6" r:id="rId6" xr:uid="{DE3DA810-BD79-0A4D-A22B-49036141AC13}"/>

</xml_diff>